<commit_message>
TODO: fix logic at end for p value
</commit_message>
<xml_diff>
--- a/Paraguay .xlsx
+++ b/Paraguay .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditya/ctc-hackathon-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E718B09E-F74D-4C46-9E2C-D80D89CCDC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93011357-F19F-F74A-A71D-4CD5639E1499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -72,6 +72,13 @@
       <sz val="10"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -116,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -141,6 +148,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -364,7 +374,7 @@
   <dimension ref="A1:W99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -376,8 +386,8 @@
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -411,8 +421,8 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
         <v>54.6</v>
       </c>
       <c r="B2" s="1">
@@ -446,8 +456,8 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
         <v>54.6</v>
       </c>
       <c r="B3" s="1">
@@ -481,8 +491,8 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
         <v>57.3</v>
       </c>
       <c r="B4" s="1">
@@ -516,8 +526,8 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
         <v>54.9</v>
       </c>
       <c r="B5" s="1">
@@ -551,8 +561,8 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
         <v>52.3</v>
       </c>
       <c r="B6" s="1">
@@ -586,8 +596,8 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
         <v>51.4</v>
       </c>
       <c r="B7" s="1">
@@ -621,8 +631,8 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
         <v>53</v>
       </c>
       <c r="B8" s="1">
@@ -656,8 +666,8 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
         <v>53</v>
       </c>
       <c r="B9" s="1">
@@ -691,8 +701,8 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
         <v>50.7</v>
       </c>
       <c r="B10" s="1">
@@ -726,8 +736,8 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
         <v>49.1</v>
       </c>
       <c r="B11" s="1">
@@ -761,8 +771,8 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
         <v>51</v>
       </c>
       <c r="B12" s="1">
@@ -796,8 +806,8 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+    <row r="13" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
         <v>52.3</v>
       </c>
       <c r="B13" s="1">
@@ -831,8 +841,8 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
         <v>47.6</v>
       </c>
       <c r="B14" s="1">
@@ -866,8 +876,8 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
         <v>47.9</v>
       </c>
       <c r="B15" s="1">
@@ -901,8 +911,8 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
         <v>50.7</v>
       </c>
       <c r="B16" s="1">
@@ -936,8 +946,8 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+    <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
         <v>47.6</v>
       </c>
       <c r="B17" s="1">
@@ -971,8 +981,8 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
         <v>47.9</v>
       </c>
       <c r="B18" s="1">
@@ -1006,8 +1016,8 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
         <v>48.5</v>
       </c>
       <c r="B19" s="1">
@@ -1041,8 +1051,8 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+    <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
         <v>46</v>
       </c>
       <c r="B20" s="1">
@@ -1076,8 +1086,8 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+    <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
         <v>45.7</v>
       </c>
       <c r="B21" s="1">
@@ -1111,7 +1121,7 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1136,7 +1146,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1161,7 +1171,7 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1186,7 +1196,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1211,7 +1221,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1236,7 +1246,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1261,7 +1271,7 @@
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1286,7 +1296,7 @@
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1311,7 +1321,7 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -1336,7 +1346,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -1361,7 +1371,7 @@
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1386,7 +1396,7 @@
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1411,7 +1421,7 @@
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1436,7 +1446,7 @@
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1461,7 +1471,7 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1486,7 +1496,7 @@
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -1511,7 +1521,7 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1536,7 +1546,7 @@
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1561,7 +1571,7 @@
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1586,7 +1596,7 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1611,7 +1621,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -1636,7 +1646,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>

</xml_diff>

<commit_message>
added two more datasets, still need to work on logic
</commit_message>
<xml_diff>
--- a/Paraguay .xlsx
+++ b/Paraguay .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditya/ctc-hackathon-2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E718B09E-F74D-4C46-9E2C-D80D89CCDC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0079A0-0590-464D-9CC5-028080390FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -72,6 +72,13 @@
       <sz val="10"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -116,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -141,6 +148,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -364,7 +374,7 @@
   <dimension ref="A1:W99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -376,8 +386,8 @@
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -411,8 +421,8 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
         <v>54.6</v>
       </c>
       <c r="B2" s="1">
@@ -446,8 +456,8 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
         <v>54.6</v>
       </c>
       <c r="B3" s="1">
@@ -481,8 +491,8 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
         <v>57.3</v>
       </c>
       <c r="B4" s="1">
@@ -516,8 +526,8 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
         <v>54.9</v>
       </c>
       <c r="B5" s="1">
@@ -551,8 +561,8 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
         <v>52.3</v>
       </c>
       <c r="B6" s="1">
@@ -586,8 +596,8 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
         <v>51.4</v>
       </c>
       <c r="B7" s="1">
@@ -621,8 +631,8 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
         <v>53</v>
       </c>
       <c r="B8" s="1">
@@ -656,8 +666,8 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
         <v>53</v>
       </c>
       <c r="B9" s="1">
@@ -691,8 +701,8 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
         <v>50.7</v>
       </c>
       <c r="B10" s="1">
@@ -726,8 +736,8 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
         <v>49.1</v>
       </c>
       <c r="B11" s="1">
@@ -761,8 +771,8 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
         <v>51</v>
       </c>
       <c r="B12" s="1">
@@ -796,8 +806,8 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+    <row r="13" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
         <v>52.3</v>
       </c>
       <c r="B13" s="1">
@@ -831,8 +841,8 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
         <v>47.6</v>
       </c>
       <c r="B14" s="1">
@@ -866,8 +876,8 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
         <v>47.9</v>
       </c>
       <c r="B15" s="1">
@@ -901,8 +911,8 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
         <v>50.7</v>
       </c>
       <c r="B16" s="1">
@@ -936,8 +946,8 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+    <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
         <v>47.6</v>
       </c>
       <c r="B17" s="1">
@@ -971,8 +981,8 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
         <v>47.9</v>
       </c>
       <c r="B18" s="1">
@@ -1006,8 +1016,8 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
         <v>48.5</v>
       </c>
       <c r="B19" s="1">
@@ -1041,8 +1051,8 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+    <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
         <v>46</v>
       </c>
       <c r="B20" s="1">
@@ -1076,8 +1086,8 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+    <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
         <v>45.7</v>
       </c>
       <c r="B21" s="1">
@@ -1111,7 +1121,7 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1136,7 +1146,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1161,7 +1171,7 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1186,7 +1196,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1211,7 +1221,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1236,7 +1246,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1261,7 +1271,7 @@
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -1286,7 +1296,7 @@
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -1311,7 +1321,7 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -1336,7 +1346,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -1361,7 +1371,7 @@
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1386,7 +1396,7 @@
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1411,7 +1421,7 @@
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -1436,7 +1446,7 @@
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1461,7 +1471,7 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1486,7 +1496,7 @@
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -1511,7 +1521,7 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1536,7 +1546,7 @@
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1561,7 +1571,7 @@
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1586,7 +1596,7 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1611,7 +1621,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -1636,7 +1646,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>

</xml_diff>